<commit_message>
Update Sprint 2 Burn-Up Chart
Shows the trend of our progress
</commit_message>
<xml_diff>
--- a/Sprint 2 Burn-Up Chart.xlsx
+++ b/Sprint 2 Burn-Up Chart.xlsx
@@ -130,12 +130,12 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -172,21 +172,21 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1954391615"/>
-        <c:axId val="1947067976"/>
+        <c:axId val="539933971"/>
+        <c:axId val="1843673634"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1954391615"/>
+        <c:axId val="539933971"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -201,10 +201,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1947067976"/>
+        <c:crossAx val="1843673634"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1947067976"/>
+        <c:axId val="1843673634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,7 +235,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1954391615"/>
+        <c:crossAx val="539933971"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -463,7 +463,9 @@
       <c r="A6" s="2">
         <v>5.0</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C6" s="4">
         <v>17.5</v>
       </c>
@@ -495,7 +497,9 @@
       <c r="A7" s="2">
         <v>6.0</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3">
+        <v>1.0</v>
+      </c>
       <c r="C7" s="4">
         <v>17.5</v>
       </c>
@@ -527,7 +531,9 @@
       <c r="A8" s="2">
         <v>7.0</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3">
+        <v>3.0</v>
+      </c>
       <c r="C8" s="4">
         <v>17.5</v>
       </c>
@@ -559,7 +565,9 @@
       <c r="A9" s="2">
         <v>8.0</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3">
+        <v>8.0</v>
+      </c>
       <c r="C9" s="4">
         <v>17.5</v>
       </c>
@@ -591,7 +599,9 @@
       <c r="A10" s="2">
         <v>9.0</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3">
+        <v>8.0</v>
+      </c>
       <c r="C10" s="4">
         <v>17.5</v>
       </c>
@@ -623,7 +633,9 @@
       <c r="A11" s="2">
         <v>10.0</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>8.0</v>
+      </c>
       <c r="C11" s="4">
         <v>17.5</v>
       </c>
@@ -655,7 +667,9 @@
       <c r="A12" s="3">
         <v>11.0</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5">
+        <v>8.0</v>
+      </c>
       <c r="C12" s="4">
         <v>17.5</v>
       </c>
@@ -687,7 +701,9 @@
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5">
+        <v>13.0</v>
+      </c>
       <c r="C13" s="4">
         <v>17.5</v>
       </c>
@@ -716,9 +732,15 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>17.5</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -744,9 +766,15 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="5">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>17.5</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -772,9 +800,15 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>17.5</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -800,9 +834,15 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="5">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>17.5</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -828,9 +868,15 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>17.5</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>

</xml_diff>

<commit_message>
New version of burnup chart
Reflected the correct chart
</commit_message>
<xml_diff>
--- a/Sprint 2 Burn-Up Chart.xlsx
+++ b/Sprint 2 Burn-Up Chart.xlsx
@@ -182,11 +182,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="539933971"/>
-        <c:axId val="1843673634"/>
+        <c:axId val="1717186552"/>
+        <c:axId val="230286379"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="539933971"/>
+        <c:axId val="1717186552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -201,10 +201,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1843673634"/>
+        <c:crossAx val="230286379"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1843673634"/>
+        <c:axId val="230286379"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,7 +235,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539933971"/>
+        <c:crossAx val="1717186552"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -257,8 +257,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -331,7 +331,7 @@
         <v>0.0</v>
       </c>
       <c r="C2" s="3">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -365,7 +365,7 @@
         <v>0.0</v>
       </c>
       <c r="C3" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -399,7 +399,7 @@
         <v>0.0</v>
       </c>
       <c r="C4" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -433,7 +433,7 @@
         <v>1.0</v>
       </c>
       <c r="C5" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -467,7 +467,7 @@
         <v>1.0</v>
       </c>
       <c r="C6" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -501,7 +501,7 @@
         <v>1.0</v>
       </c>
       <c r="C7" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -535,7 +535,7 @@
         <v>3.0</v>
       </c>
       <c r="C8" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -569,7 +569,7 @@
         <v>8.0</v>
       </c>
       <c r="C9" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -603,7 +603,7 @@
         <v>8.0</v>
       </c>
       <c r="C10" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -637,7 +637,7 @@
         <v>8.0</v>
       </c>
       <c r="C11" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -671,7 +671,7 @@
         <v>8.0</v>
       </c>
       <c r="C12" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -705,7 +705,7 @@
         <v>13.0</v>
       </c>
       <c r="C13" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -739,7 +739,7 @@
         <v>13.0</v>
       </c>
       <c r="C14" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -773,7 +773,7 @@
         <v>13.0</v>
       </c>
       <c r="C15" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -807,7 +807,7 @@
         <v>13.0</v>
       </c>
       <c r="C16" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -841,7 +841,7 @@
         <v>17.0</v>
       </c>
       <c r="C17" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -872,10 +872,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="5">
-        <v>17.5</v>
+        <v>22.0</v>
       </c>
       <c r="C18" s="4">
-        <v>17.5</v>
+        <v>30.5</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>

</xml_diff>